<commit_message>
update binary files for client and contract insert success and transform data
</commit_message>
<xml_diff>
--- a/src/inserted/cliente_insert_sucess.xlsx
+++ b/src/inserted/cliente_insert_sucess.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,75 +436,80 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>razaoSocial</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Email</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Celular</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>cpf_cnpj</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>rg_ie</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>filial_id</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>idCidade</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Endereco</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Complemento</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Numero</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Bairro</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Cep</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>idClienteIXC</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>statusInsercao</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>logRetorno</t>
         </is>
@@ -516,77 +521,82 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>1306</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>Abelanio Veríssimo Peixoto</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>teste@gmail.com</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>99999999999</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>014.846.390-81</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>Isento</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>35</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>1659</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>Vila São Sebastião</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>Próximo ao cacimbão</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="L2" t="inlineStr">
         <is>
+          <t>SN</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
           <t>Centro</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>57830-000</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>117693</t>
-        </is>
-      </c>
       <c r="O2" t="inlineStr">
         <is>
+          <t>117695</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
           <t>sucesso</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>{'type': 'success', 'message': 'Registro inserido com sucesso!', 'id': '117693', 'atualiza_campos': [{'tipo': 'r', 'campo': 'ativo', 'valor': 'S'}, {'tipo': 'i', 'campo': 'data_cadastro', 'valor': '19/03/2025'}, {'tipo': 'i', 'campo': 'filial_id', 'valor': '35'}, {'tipo': 'i', 'campo': 'latitude', 'valor': ''}, {'tipo': 'i', 'campo': 'longitude', 'valor': ''}, {'tipo': 'i', 'campo': 'id_conta', 'valor': '919704'}, {'tipo': 'd', 'campo': 'crm_data_vencemos', 'valor': ''}, {'tipo': 'r', 'campo': 'convert_cliente_forn', 'valor': ''}, {'tipo': 'd', 'campo': 'crm_data_perdemos', 'valor': ''}, {'tipo': 'i', 'campo': 'crm_data_sem_viabilidade', 'valor': ''}, {'tipo': 'i', 'campo': 'crm_data_sem_porta_disponivel', 'valor': ''}, {'tipo': 'i', 'campo': 'crm_data_abortamos', 'valor': ''}, {'tipo': 'i', 'campo': 'crm_data_negociando', 'valor': ''}, {'tipo': 'i', 'campo': 'crm_data_apresentando', 'valor': ''}, {'tipo': 'i', 'campo': 'crm_data_sondagem', 'valor': ''}, {'tipo': 'i', 'campo': 'crm_data_novo', 'valor': ''}]}</t>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>{'type': 'success', 'message': 'Registro inserido com sucesso!', 'id': '117695', 'atualiza_campos': [{'tipo': 'r', 'campo': 'ativo', 'valor': 'S'}, {'tipo': 'i', 'campo': 'data_cadastro', 'valor': '19/03/2025'}, {'tipo': 'i', 'campo': 'filial_id', 'valor': '35'}, {'tipo': 'i', 'campo': 'latitude', 'valor': ''}, {'tipo': 'i', 'campo': 'longitude', 'valor': ''}, {'tipo': 'i', 'campo': 'id_conta', 'valor': '919706'}, {'tipo': 'd', 'campo': 'crm_data_vencemos', 'valor': ''}, {'tipo': 'r', 'campo': 'convert_cliente_forn', 'valor': ''}, {'tipo': 'd', 'campo': 'crm_data_perdemos', 'valor': ''}, {'tipo': 'i', 'campo': 'crm_data_sem_viabilidade', 'valor': ''}, {'tipo': 'i', 'campo': 'crm_data_sem_porta_disponivel', 'valor': ''}, {'tipo': 'i', 'campo': 'crm_data_abortamos', 'valor': ''}, {'tipo': 'i', 'campo': 'crm_data_negociando', 'valor': ''}, {'tipo': 'i', 'campo': 'crm_data_apresentando', 'valor': ''}, {'tipo': 'i', 'campo': 'crm_data_sondagem', 'valor': ''}, {'tipo': 'i', 'campo': 'crm_data_novo', 'valor': ''}]}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
remove unused code cell from insert_client notebook and update binary files
</commit_message>
<xml_diff>
--- a/src/inserted/cliente_insert_sucess.xlsx
+++ b/src/inserted/cliente_insert_sucess.xlsx
@@ -586,7 +586,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>117695</t>
+          <t>117696</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -596,7 +596,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>{'type': 'success', 'message': 'Registro inserido com sucesso!', 'id': '117695', 'atualiza_campos': [{'tipo': 'r', 'campo': 'ativo', 'valor': 'S'}, {'tipo': 'i', 'campo': 'data_cadastro', 'valor': '19/03/2025'}, {'tipo': 'i', 'campo': 'filial_id', 'valor': '35'}, {'tipo': 'i', 'campo': 'latitude', 'valor': ''}, {'tipo': 'i', 'campo': 'longitude', 'valor': ''}, {'tipo': 'i', 'campo': 'id_conta', 'valor': '919706'}, {'tipo': 'd', 'campo': 'crm_data_vencemos', 'valor': ''}, {'tipo': 'r', 'campo': 'convert_cliente_forn', 'valor': ''}, {'tipo': 'd', 'campo': 'crm_data_perdemos', 'valor': ''}, {'tipo': 'i', 'campo': 'crm_data_sem_viabilidade', 'valor': ''}, {'tipo': 'i', 'campo': 'crm_data_sem_porta_disponivel', 'valor': ''}, {'tipo': 'i', 'campo': 'crm_data_abortamos', 'valor': ''}, {'tipo': 'i', 'campo': 'crm_data_negociando', 'valor': ''}, {'tipo': 'i', 'campo': 'crm_data_apresentando', 'valor': ''}, {'tipo': 'i', 'campo': 'crm_data_sondagem', 'valor': ''}, {'tipo': 'i', 'campo': 'crm_data_novo', 'valor': ''}]}</t>
+          <t>{'type': 'success', 'message': 'Registro inserido com sucesso!', 'id': '117696', 'atualiza_campos': [{'tipo': 'r', 'campo': 'ativo', 'valor': 'S'}, {'tipo': 'i', 'campo': 'data_cadastro', 'valor': '19/03/2025'}, {'tipo': 'i', 'campo': 'filial_id', 'valor': '35'}, {'tipo': 'i', 'campo': 'latitude', 'valor': ''}, {'tipo': 'i', 'campo': 'longitude', 'valor': ''}, {'tipo': 'i', 'campo': 'id_conta', 'valor': '919707'}, {'tipo': 'd', 'campo': 'crm_data_vencemos', 'valor': ''}, {'tipo': 'r', 'campo': 'convert_cliente_forn', 'valor': ''}, {'tipo': 'd', 'campo': 'crm_data_perdemos', 'valor': ''}, {'tipo': 'i', 'campo': 'crm_data_sem_viabilidade', 'valor': ''}, {'tipo': 'i', 'campo': 'crm_data_sem_porta_disponivel', 'valor': ''}, {'tipo': 'i', 'campo': 'crm_data_abortamos', 'valor': ''}, {'tipo': 'i', 'campo': 'crm_data_negociando', 'valor': ''}, {'tipo': 'i', 'campo': 'crm_data_apresentando', 'valor': ''}, {'tipo': 'i', 'campo': 'crm_data_sondagem', 'valor': ''}, {'tipo': 'i', 'campo': 'crm_data_novo', 'valor': ''}]}</t>
         </is>
       </c>
     </row>

</xml_diff>